<commit_message>
carrega dados detalhados dos instrumentos e regera o json
</commit_message>
<xml_diff>
--- a/R/dados_instrumentos.xlsx
+++ b/R/dados_instrumentos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiago/Documents/github/timeline-covid/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B9839D-6B04-2A4F-A2A7-58CE7E422745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFFD5FC8-58BB-594E-85ED-07FDD88F2F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="1620" windowWidth="25440" windowHeight="12820" xr2:uid="{69F0099A-28B2-B64C-97C8-E3F59C51DA57}"/>
+    <workbookView xWindow="-35500" yWindow="2280" windowWidth="25440" windowHeight="12820" xr2:uid="{69F0099A-28B2-B64C-97C8-E3F59C51DA57}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="211">
   <si>
     <t>http://www.planalto.gov.br/CCIVIL_03/_Ato2019-2022/2020/Mpv/mpv929.htm</t>
   </si>
@@ -642,7 +642,31 @@
     <t>data</t>
   </si>
   <si>
-    <t>anotação</t>
+    <t>anotacao</t>
+  </si>
+  <si>
+    <t>anotacao_fixa</t>
+  </si>
+  <si>
+    <t>Operação regresso de brasileiros no exterior</t>
+  </si>
+  <si>
+    <t>Aquisição de EPIs e capacitação para conter danos da pandemia global</t>
+  </si>
+  <si>
+    <t>Auxílio Emergencial</t>
+  </si>
+  <si>
+    <t>Programa Federativo de Enfrentamento ao Coronavírus: suspensão da dívida e auxílio financeiro aos entes</t>
+  </si>
+  <si>
+    <t>Garantir ações necessárias à produção e disponibilização de possível vacina</t>
+  </si>
+  <si>
+    <t>Auxílio Setor Cultural</t>
+  </si>
+  <si>
+    <t>Auxílio Emergencial no valor de R$ 300</t>
   </si>
 </sst>
 </file>
@@ -1075,10 +1099,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7317090F-0B1F-F145-98D4-DA3D2D7A452A}">
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1086,13 +1110,14 @@
     <col min="1" max="1" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="69.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="88" style="3" customWidth="1"/>
-    <col min="6" max="6" width="86.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="19" style="3" customWidth="1"/>
+    <col min="5" max="5" width="69.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="88" style="3" customWidth="1"/>
+    <col min="7" max="7" width="86.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>199</v>
       </c>
@@ -1103,16 +1128,19 @@
         <v>201</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -1122,17 +1150,18 @@
       <c r="C2" s="5">
         <v>43915</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5"/>
+      <c r="E2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -1142,17 +1171,18 @@
       <c r="C3" s="5">
         <v>43923</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -1162,17 +1192,20 @@
       <c r="C4" s="5">
         <v>43923</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -1182,17 +1215,18 @@
       <c r="C5" s="5">
         <v>43929</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="5"/>
+      <c r="E5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="G5" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -1202,17 +1236,18 @@
       <c r="C6" s="5">
         <v>43929</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="5"/>
+      <c r="E6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="G6" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -1222,17 +1257,18 @@
       <c r="C7" s="9">
         <v>43936</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="9"/>
+      <c r="E7" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="F7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="G7" s="10" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -1242,17 +1278,18 @@
       <c r="C8" s="9">
         <v>43945</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="9"/>
+      <c r="E8" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="G8" s="10" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -1262,17 +1299,18 @@
       <c r="C9" s="9">
         <v>43976</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="9"/>
+      <c r="E9" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="F9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="G9" s="10" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1282,17 +1320,18 @@
       <c r="C10" s="9">
         <v>44012</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="9"/>
+      <c r="E10" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="F10" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="G10" s="10" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1302,17 +1341,20 @@
       <c r="C11" s="9">
         <v>44021</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="F11" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="G11" s="10" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -1322,17 +1364,20 @@
       <c r="C12" s="9">
         <v>44076</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="F12" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="G12" s="10" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
@@ -1342,17 +1387,18 @@
       <c r="C13" s="9">
         <v>44130</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="9"/>
+      <c r="E13" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="F13" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="G13" s="10" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -1362,17 +1408,20 @@
       <c r="C14" s="9">
         <v>44273</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="F14" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="G14" s="10" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1382,17 +1431,18 @@
       <c r="C15" s="9">
         <v>44273</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="9"/>
+      <c r="E15" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="F15" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="G15" s="10" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>44</v>
       </c>
@@ -1402,17 +1452,20 @@
       <c r="C16" s="5">
         <v>43922</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="F16" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="G16" s="7" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>44</v>
       </c>
@@ -1422,17 +1475,18 @@
       <c r="C17" s="5">
         <v>43924</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="5"/>
+      <c r="E17" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="F17" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="G17" s="7" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>44</v>
       </c>
@@ -1442,17 +1496,18 @@
       <c r="C18" s="5">
         <v>43924</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="5"/>
+      <c r="E18" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="F18" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="G18" s="7" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>44</v>
       </c>
@@ -1462,17 +1517,18 @@
       <c r="C19" s="5">
         <v>43945</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="5"/>
+      <c r="E19" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="F19" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="G19" s="7" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>44</v>
       </c>
@@ -1482,17 +1538,18 @@
       <c r="C20" s="5">
         <v>43958</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="5"/>
+      <c r="E20" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="F20" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="G20" s="7" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>44</v>
       </c>
@@ -1502,17 +1559,18 @@
       <c r="C21" s="5">
         <v>43977</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="5"/>
+      <c r="E21" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="F21" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="G21" s="7" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>44</v>
       </c>
@@ -1522,17 +1580,18 @@
       <c r="C22" s="5">
         <v>43986</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="5"/>
+      <c r="E22" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="F22" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="G22" s="7" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>44</v>
       </c>
@@ -1542,17 +1601,18 @@
       <c r="C23" s="5">
         <v>44027</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="5"/>
+      <c r="E23" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="F23" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="G23" s="7" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>44</v>
       </c>
@@ -1562,17 +1622,18 @@
       <c r="C24" s="5">
         <v>44074</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="5"/>
+      <c r="E24" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="F24" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="G24" s="7" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>44</v>
       </c>
@@ -1582,17 +1643,18 @@
       <c r="C25" s="12">
         <v>44089</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="12"/>
+      <c r="E25" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="F25" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="F25" s="13" t="s">
+      <c r="G25" s="13" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>44</v>
       </c>
@@ -1602,17 +1664,18 @@
       <c r="C26" s="5">
         <v>44097</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="5"/>
+      <c r="E26" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="F26" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="G26" s="7" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>44</v>
       </c>
@@ -1622,17 +1685,18 @@
       <c r="C27" s="5">
         <v>44194</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="5"/>
+      <c r="E27" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="F27" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="G27" s="7" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>44</v>
       </c>
@@ -1642,17 +1706,18 @@
       <c r="C28" s="5">
         <v>44313</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="5"/>
+      <c r="E28" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="F28" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="G28" s="7" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>81</v>
       </c>
@@ -1662,17 +1727,18 @@
       <c r="C29" s="9">
         <v>43923</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="9"/>
+      <c r="E29" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E29" s="14" t="s">
+      <c r="F29" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="G29" s="10" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>81</v>
       </c>
@@ -1682,17 +1748,18 @@
       <c r="C30" s="9">
         <v>43923</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="9"/>
+      <c r="E30" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E30" s="14" t="s">
+      <c r="F30" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="F30" s="10" t="s">
+      <c r="G30" s="10" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>81</v>
       </c>
@@ -1702,17 +1769,20 @@
       <c r="C31" s="9">
         <v>43978</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="E31" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E31" s="14" t="s">
+      <c r="F31" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="F31" s="10" t="s">
+      <c r="G31" s="10" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>81</v>
       </c>
@@ -1722,17 +1792,18 @@
       <c r="C32" s="9">
         <v>43986</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="9"/>
+      <c r="E32" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="F32" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="G32" s="10" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>94</v>
       </c>
@@ -1742,17 +1813,20 @@
       <c r="C33" s="9">
         <v>43868</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="E33" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="F33" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="F33" s="7" t="s">
+      <c r="G33" s="7" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>94</v>
       </c>
@@ -1762,17 +1836,20 @@
       <c r="C34" s="9">
         <v>43903</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="E34" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="F34" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="G34" s="7" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>94</v>
       </c>
@@ -1782,17 +1859,20 @@
       <c r="C35" s="9">
         <v>43915</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="E35" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="E35" s="14" t="s">
+      <c r="F35" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F35" s="15" t="s">
+      <c r="G35" s="15" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
         <v>94</v>
       </c>
@@ -1802,17 +1882,18 @@
       <c r="C36" s="9">
         <v>43923</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="9"/>
+      <c r="E36" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="E36" s="14" t="s">
+      <c r="F36" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="F36" s="7" t="s">
+      <c r="G36" s="7" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>94</v>
       </c>
@@ -1822,17 +1903,18 @@
       <c r="C37" s="9">
         <v>43923</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="9"/>
+      <c r="E37" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="E37" s="14" t="s">
+      <c r="F37" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="F37" s="13" t="s">
+      <c r="G37" s="13" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>94</v>
       </c>
@@ -1842,17 +1924,18 @@
       <c r="C38" s="9">
         <v>43923</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="9"/>
+      <c r="E38" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="E38" s="14" t="s">
+      <c r="F38" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="F38" s="13" t="s">
+      <c r="G38" s="13" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>94</v>
       </c>
@@ -1862,17 +1945,18 @@
       <c r="C39" s="9">
         <v>43929</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="9"/>
+      <c r="E39" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="E39" s="14" t="s">
+      <c r="F39" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="F39" s="7" t="s">
+      <c r="G39" s="7" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>94</v>
       </c>
@@ -1882,17 +1966,18 @@
       <c r="C40" s="9">
         <v>43936</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D40" s="9"/>
+      <c r="E40" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="E40" s="14" t="s">
+      <c r="F40" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="F40" s="13" t="s">
+      <c r="G40" s="13" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>94</v>
       </c>
@@ -1902,17 +1987,18 @@
       <c r="C41" s="9">
         <v>43957</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D41" s="9"/>
+      <c r="E41" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="E41" s="14" t="s">
+      <c r="F41" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="F41" s="15" t="s">
+      <c r="G41" s="15" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>94</v>
       </c>
@@ -1922,17 +2008,18 @@
       <c r="C42" s="9">
         <v>43964</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D42" s="9"/>
+      <c r="E42" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="E42" s="14" t="s">
+      <c r="F42" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="F42" s="7" t="s">
+      <c r="G42" s="7" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
         <v>94</v>
       </c>
@@ -1942,17 +2029,18 @@
       <c r="C43" s="9">
         <v>43970</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="9"/>
+      <c r="E43" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="E43" s="14" t="s">
+      <c r="F43" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="F43" s="7" t="s">
+      <c r="G43" s="7" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
         <v>94</v>
       </c>
@@ -1962,17 +2050,18 @@
       <c r="C44" s="9">
         <v>43971</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="D44" s="9"/>
+      <c r="E44" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="E44" s="14" t="s">
+      <c r="F44" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="F44" s="7" t="s">
+      <c r="G44" s="7" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
         <v>94</v>
       </c>
@@ -1982,17 +2071,18 @@
       <c r="C45" s="9">
         <v>43976</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D45" s="9"/>
+      <c r="E45" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E45" s="14" t="s">
+      <c r="F45" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F45" s="7" t="s">
+      <c r="G45" s="7" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
         <v>94</v>
       </c>
@@ -2002,17 +2092,18 @@
       <c r="C46" s="9">
         <v>43986</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D46" s="9"/>
+      <c r="E46" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="E46" s="14" t="s">
+      <c r="F46" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="F46" s="7" t="s">
+      <c r="G46" s="7" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>94</v>
       </c>
@@ -2022,17 +2113,18 @@
       <c r="C47" s="9">
         <v>44007</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="D47" s="9"/>
+      <c r="E47" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="E47" s="14" t="s">
+      <c r="F47" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="F47" s="7" t="s">
+      <c r="G47" s="7" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
         <v>94</v>
       </c>
@@ -2042,17 +2134,18 @@
       <c r="C48" s="9">
         <v>44020</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="D48" s="9"/>
+      <c r="E48" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="E48" s="14" t="s">
+      <c r="F48" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="F48" s="7" t="s">
+      <c r="G48" s="7" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
         <v>94</v>
       </c>
@@ -2062,17 +2155,20 @@
       <c r="C49" s="9">
         <v>44049</v>
       </c>
-      <c r="D49" s="8" t="s">
+      <c r="D49" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="E49" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="E49" s="14" t="s">
+      <c r="F49" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="F49" s="7" t="s">
+      <c r="G49" s="7" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
         <v>94</v>
       </c>
@@ -2082,17 +2178,18 @@
       <c r="C50" s="9">
         <v>44098</v>
       </c>
-      <c r="D50" s="8" t="s">
+      <c r="D50" s="9"/>
+      <c r="E50" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="E50" s="14" t="s">
+      <c r="F50" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="F50" s="7" t="s">
+      <c r="G50" s="7" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
         <v>94</v>
       </c>
@@ -2102,17 +2199,18 @@
       <c r="C51" s="9">
         <v>44106</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="D51" s="9"/>
+      <c r="E51" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="E51" s="14" t="s">
+      <c r="F51" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="F51" s="7" t="s">
+      <c r="G51" s="7" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
         <v>94</v>
       </c>
@@ -2122,17 +2220,18 @@
       <c r="C52" s="9">
         <v>44182</v>
       </c>
-      <c r="D52" s="8" t="s">
+      <c r="D52" s="9"/>
+      <c r="E52" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="E52" s="14" t="s">
+      <c r="F52" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="F52" s="7" t="s">
+      <c r="G52" s="7" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
         <v>94</v>
       </c>
@@ -2142,17 +2241,18 @@
       <c r="C53" s="9">
         <v>44251</v>
       </c>
-      <c r="D53" s="8" t="s">
+      <c r="D53" s="9"/>
+      <c r="E53" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="E53" s="14" t="s">
+      <c r="F53" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="F53" s="7" t="s">
+      <c r="G53" s="7" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
         <v>94</v>
       </c>
@@ -2162,17 +2262,18 @@
       <c r="C54" s="9">
         <v>44285</v>
       </c>
-      <c r="D54" s="8" t="s">
+      <c r="D54" s="9"/>
+      <c r="E54" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="E54" s="14" t="s">
+      <c r="F54" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="F54" s="7" t="s">
+      <c r="G54" s="7" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
         <v>94</v>
       </c>
@@ -2182,17 +2283,18 @@
       <c r="C55" s="9">
         <v>44302</v>
       </c>
-      <c r="D55" s="8" t="s">
+      <c r="D55" s="9"/>
+      <c r="E55" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="E55" s="14" t="s">
+      <c r="F55" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="F55" s="7" t="s">
+      <c r="G55" s="7" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
         <v>94</v>
       </c>
@@ -2202,84 +2304,88 @@
       <c r="C56" s="9">
         <v>44326</v>
       </c>
-      <c r="D56" s="8" t="s">
+      <c r="D56" s="9"/>
+      <c r="E56" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="E56" s="14" t="s">
+      <c r="F56" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="F56" s="7" t="s">
+      <c r="G56" s="7" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="7"/>
       <c r="B57" s="10"/>
       <c r="C57" s="9"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D57" s="9"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="7"/>
       <c r="B58" s="10"/>
       <c r="C58" s="9"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D58" s="9"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="7"/>
       <c r="B59" s="10"/>
       <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D7" r:id="rId1" xr:uid="{461C50D3-8598-F346-967F-16C34F983E27}"/>
-    <hyperlink ref="D8" r:id="rId2" xr:uid="{B32E26A4-FED2-D54D-9390-061A2B86883D}"/>
-    <hyperlink ref="D9" r:id="rId3" xr:uid="{8FB87534-8637-954E-94E0-F3A0C0D1C296}"/>
-    <hyperlink ref="D10" r:id="rId4" xr:uid="{827234E4-584A-D042-8FD6-2D2663CDCAD3}"/>
-    <hyperlink ref="D11" r:id="rId5" xr:uid="{5756EC77-05B7-4643-8B9B-BBA3783D1903}"/>
-    <hyperlink ref="D12" r:id="rId6" xr:uid="{35F7DA24-43C2-1043-8D31-5A3AAE0AD1CA}"/>
-    <hyperlink ref="D13" r:id="rId7" xr:uid="{2563F805-6157-0347-8FE5-90E68EE6D394}"/>
-    <hyperlink ref="D14" r:id="rId8" xr:uid="{C51F883F-84C7-CE46-B297-3B80EC27372F}"/>
-    <hyperlink ref="D15" r:id="rId9" xr:uid="{1AE0120B-AE00-0E40-92CA-6662900361B7}"/>
-    <hyperlink ref="D16" r:id="rId10" xr:uid="{30FAB9B8-C3DE-C74E-9EDB-CDB9469E076F}"/>
-    <hyperlink ref="D17" r:id="rId11" xr:uid="{1AFE0CD4-1DC5-284E-AE79-2B5517C4AC31}"/>
-    <hyperlink ref="D18" r:id="rId12" xr:uid="{ACF6B6CC-7449-7545-9871-2ADBF14E6B47}"/>
-    <hyperlink ref="D19" r:id="rId13" xr:uid="{FA7A847F-79DE-2843-B309-056697AEC177}"/>
-    <hyperlink ref="D20" r:id="rId14" xr:uid="{CA729DA7-5D78-5B49-B4AF-907D829008ED}"/>
-    <hyperlink ref="D21" r:id="rId15" xr:uid="{7CEF3280-ED4C-C443-BD6B-19E322339FDA}"/>
-    <hyperlink ref="D22" r:id="rId16" xr:uid="{3A85F5AD-30BF-8248-883B-3B15D92916B6}"/>
-    <hyperlink ref="D23" r:id="rId17" xr:uid="{A86B9479-3DD2-DF43-BF55-11EB3E20CBEF}"/>
-    <hyperlink ref="D24" r:id="rId18" xr:uid="{76DB6588-FC85-CB4D-BF7F-28C4896BCEBB}"/>
-    <hyperlink ref="D25" r:id="rId19" xr:uid="{9F94145B-5903-9B4F-968C-4F42794B90B5}"/>
-    <hyperlink ref="D26" r:id="rId20" xr:uid="{D8FA5E39-489B-0849-8121-3FC2A5355834}"/>
-    <hyperlink ref="D27" r:id="rId21" xr:uid="{60854075-DD60-BF42-9A57-FC32ABE25DD9}"/>
-    <hyperlink ref="D28" r:id="rId22" xr:uid="{A6A3A017-408F-2E41-B0FB-1DD7C6BC6379}"/>
-    <hyperlink ref="D29" r:id="rId23" xr:uid="{F267FD6F-9D17-BF43-BB46-4A13FEB78780}"/>
-    <hyperlink ref="D30" r:id="rId24" xr:uid="{DF58CA40-EDF6-6F4A-AE9E-D31B30CFAB46}"/>
-    <hyperlink ref="D31" r:id="rId25" xr:uid="{32156FE5-1D00-BB43-A137-57BF36B23282}"/>
-    <hyperlink ref="D32" r:id="rId26" xr:uid="{D99DB1CB-2D16-BA44-860A-8B80D36FDD01}"/>
-    <hyperlink ref="D33" r:id="rId27" xr:uid="{45DEC6D6-3058-084E-AB97-A541D6F030D5}"/>
-    <hyperlink ref="D34" r:id="rId28" xr:uid="{56AE25B0-3BE6-CC4C-AC50-A98F5E12D60D}"/>
-    <hyperlink ref="D35" r:id="rId29" xr:uid="{41F4236B-18FA-8B48-9DA1-4E55ECF05EA5}"/>
-    <hyperlink ref="D36" r:id="rId30" xr:uid="{14B4F66D-D1F0-984B-81E2-CA9BFDC9D271}"/>
-    <hyperlink ref="D37" r:id="rId31" xr:uid="{F00A879D-A2FB-364A-9048-6DD554B724FC}"/>
-    <hyperlink ref="D38" r:id="rId32" xr:uid="{4562FC19-17B8-8144-BACB-559D2D30CABF}"/>
-    <hyperlink ref="D39" r:id="rId33" xr:uid="{FF19A9DE-583F-2840-8464-54354FCFDCF8}"/>
-    <hyperlink ref="D40" r:id="rId34" xr:uid="{1DF1877E-D6DA-7042-92F7-77E94B428045}"/>
-    <hyperlink ref="D41" r:id="rId35" xr:uid="{0BA585E2-E0EB-9B4D-878C-9D89A101A7E8}"/>
-    <hyperlink ref="D42" r:id="rId36" xr:uid="{FA709120-9F20-6147-8D8B-BF9C1EB2E28A}"/>
-    <hyperlink ref="D43" r:id="rId37" xr:uid="{E70DF94B-0EB3-104A-8B78-8841FA2F9B12}"/>
-    <hyperlink ref="D44" r:id="rId38" xr:uid="{41BCF087-4C90-7241-AD45-FA8464AE7350}"/>
-    <hyperlink ref="D45" r:id="rId39" xr:uid="{AC529185-B855-1648-8B4C-8A8D905AFE49}"/>
-    <hyperlink ref="D46" r:id="rId40" xr:uid="{5066A69F-1E3E-3F41-AE26-92EE4316B3B9}"/>
-    <hyperlink ref="D47" r:id="rId41" xr:uid="{362F4020-DD92-154F-ACDA-76602A2A6759}"/>
-    <hyperlink ref="D48" r:id="rId42" xr:uid="{383C0426-1F8F-2147-85C0-357034B3A9B5}"/>
-    <hyperlink ref="D49" r:id="rId43" xr:uid="{A25C3C3F-0E65-8E43-AC71-68ED62A9D49B}"/>
-    <hyperlink ref="D50" r:id="rId44" xr:uid="{DE69892C-E409-4E44-A83B-8C32077772E2}"/>
-    <hyperlink ref="D51" r:id="rId45" xr:uid="{E1A5ED49-C6D3-594F-A47A-B9E06C7A9988}"/>
-    <hyperlink ref="D52" r:id="rId46" xr:uid="{0BF898E7-7E98-C444-A45C-4E387230E9BE}"/>
-    <hyperlink ref="D53" r:id="rId47" xr:uid="{209981A1-9E1D-DD41-9FDC-774DFCD17AD3}"/>
-    <hyperlink ref="D54" r:id="rId48" xr:uid="{01F83B42-417B-7E49-8E45-ADEC9E0C5C19}"/>
-    <hyperlink ref="D55" r:id="rId49" xr:uid="{A0BDFFED-5387-0F4C-9884-246C2DF53CD2}"/>
-    <hyperlink ref="D56" r:id="rId50" xr:uid="{D20543E9-DE50-EF44-ADCC-FE4E49F5B868}"/>
-    <hyperlink ref="D6" r:id="rId51" xr:uid="{D17F2BE4-9635-C146-8619-9BF315E32413}"/>
+    <hyperlink ref="E7" r:id="rId1" xr:uid="{461C50D3-8598-F346-967F-16C34F983E27}"/>
+    <hyperlink ref="E8" r:id="rId2" xr:uid="{B32E26A4-FED2-D54D-9390-061A2B86883D}"/>
+    <hyperlink ref="E9" r:id="rId3" xr:uid="{8FB87534-8637-954E-94E0-F3A0C0D1C296}"/>
+    <hyperlink ref="E10" r:id="rId4" xr:uid="{827234E4-584A-D042-8FD6-2D2663CDCAD3}"/>
+    <hyperlink ref="E11" r:id="rId5" xr:uid="{5756EC77-05B7-4643-8B9B-BBA3783D1903}"/>
+    <hyperlink ref="E12" r:id="rId6" xr:uid="{35F7DA24-43C2-1043-8D31-5A3AAE0AD1CA}"/>
+    <hyperlink ref="E13" r:id="rId7" xr:uid="{2563F805-6157-0347-8FE5-90E68EE6D394}"/>
+    <hyperlink ref="E14" r:id="rId8" xr:uid="{C51F883F-84C7-CE46-B297-3B80EC27372F}"/>
+    <hyperlink ref="E15" r:id="rId9" xr:uid="{1AE0120B-AE00-0E40-92CA-6662900361B7}"/>
+    <hyperlink ref="E16" r:id="rId10" xr:uid="{30FAB9B8-C3DE-C74E-9EDB-CDB9469E076F}"/>
+    <hyperlink ref="E17" r:id="rId11" xr:uid="{1AFE0CD4-1DC5-284E-AE79-2B5517C4AC31}"/>
+    <hyperlink ref="E18" r:id="rId12" xr:uid="{ACF6B6CC-7449-7545-9871-2ADBF14E6B47}"/>
+    <hyperlink ref="E19" r:id="rId13" xr:uid="{FA7A847F-79DE-2843-B309-056697AEC177}"/>
+    <hyperlink ref="E20" r:id="rId14" xr:uid="{CA729DA7-5D78-5B49-B4AF-907D829008ED}"/>
+    <hyperlink ref="E21" r:id="rId15" xr:uid="{7CEF3280-ED4C-C443-BD6B-19E322339FDA}"/>
+    <hyperlink ref="E22" r:id="rId16" xr:uid="{3A85F5AD-30BF-8248-883B-3B15D92916B6}"/>
+    <hyperlink ref="E23" r:id="rId17" xr:uid="{A86B9479-3DD2-DF43-BF55-11EB3E20CBEF}"/>
+    <hyperlink ref="E24" r:id="rId18" xr:uid="{76DB6588-FC85-CB4D-BF7F-28C4896BCEBB}"/>
+    <hyperlink ref="E25" r:id="rId19" xr:uid="{9F94145B-5903-9B4F-968C-4F42794B90B5}"/>
+    <hyperlink ref="E26" r:id="rId20" xr:uid="{D8FA5E39-489B-0849-8121-3FC2A5355834}"/>
+    <hyperlink ref="E27" r:id="rId21" xr:uid="{60854075-DD60-BF42-9A57-FC32ABE25DD9}"/>
+    <hyperlink ref="E28" r:id="rId22" xr:uid="{A6A3A017-408F-2E41-B0FB-1DD7C6BC6379}"/>
+    <hyperlink ref="E29" r:id="rId23" xr:uid="{F267FD6F-9D17-BF43-BB46-4A13FEB78780}"/>
+    <hyperlink ref="E30" r:id="rId24" xr:uid="{DF58CA40-EDF6-6F4A-AE9E-D31B30CFAB46}"/>
+    <hyperlink ref="E31" r:id="rId25" xr:uid="{32156FE5-1D00-BB43-A137-57BF36B23282}"/>
+    <hyperlink ref="E32" r:id="rId26" xr:uid="{D99DB1CB-2D16-BA44-860A-8B80D36FDD01}"/>
+    <hyperlink ref="E33" r:id="rId27" xr:uid="{45DEC6D6-3058-084E-AB97-A541D6F030D5}"/>
+    <hyperlink ref="E34" r:id="rId28" xr:uid="{56AE25B0-3BE6-CC4C-AC50-A98F5E12D60D}"/>
+    <hyperlink ref="E35" r:id="rId29" xr:uid="{41F4236B-18FA-8B48-9DA1-4E55ECF05EA5}"/>
+    <hyperlink ref="E36" r:id="rId30" xr:uid="{14B4F66D-D1F0-984B-81E2-CA9BFDC9D271}"/>
+    <hyperlink ref="E37" r:id="rId31" xr:uid="{F00A879D-A2FB-364A-9048-6DD554B724FC}"/>
+    <hyperlink ref="E38" r:id="rId32" xr:uid="{4562FC19-17B8-8144-BACB-559D2D30CABF}"/>
+    <hyperlink ref="E39" r:id="rId33" xr:uid="{FF19A9DE-583F-2840-8464-54354FCFDCF8}"/>
+    <hyperlink ref="E40" r:id="rId34" xr:uid="{1DF1877E-D6DA-7042-92F7-77E94B428045}"/>
+    <hyperlink ref="E41" r:id="rId35" xr:uid="{0BA585E2-E0EB-9B4D-878C-9D89A101A7E8}"/>
+    <hyperlink ref="E42" r:id="rId36" xr:uid="{FA709120-9F20-6147-8D8B-BF9C1EB2E28A}"/>
+    <hyperlink ref="E43" r:id="rId37" xr:uid="{E70DF94B-0EB3-104A-8B78-8841FA2F9B12}"/>
+    <hyperlink ref="E44" r:id="rId38" xr:uid="{41BCF087-4C90-7241-AD45-FA8464AE7350}"/>
+    <hyperlink ref="E45" r:id="rId39" xr:uid="{AC529185-B855-1648-8B4C-8A8D905AFE49}"/>
+    <hyperlink ref="E46" r:id="rId40" xr:uid="{5066A69F-1E3E-3F41-AE26-92EE4316B3B9}"/>
+    <hyperlink ref="E47" r:id="rId41" xr:uid="{362F4020-DD92-154F-ACDA-76602A2A6759}"/>
+    <hyperlink ref="E48" r:id="rId42" xr:uid="{383C0426-1F8F-2147-85C0-357034B3A9B5}"/>
+    <hyperlink ref="E49" r:id="rId43" xr:uid="{A25C3C3F-0E65-8E43-AC71-68ED62A9D49B}"/>
+    <hyperlink ref="E50" r:id="rId44" xr:uid="{DE69892C-E409-4E44-A83B-8C32077772E2}"/>
+    <hyperlink ref="E51" r:id="rId45" xr:uid="{E1A5ED49-C6D3-594F-A47A-B9E06C7A9988}"/>
+    <hyperlink ref="E52" r:id="rId46" xr:uid="{0BF898E7-7E98-C444-A45C-4E387230E9BE}"/>
+    <hyperlink ref="E53" r:id="rId47" xr:uid="{209981A1-9E1D-DD41-9FDC-774DFCD17AD3}"/>
+    <hyperlink ref="E54" r:id="rId48" xr:uid="{01F83B42-417B-7E49-8E45-ADEC9E0C5C19}"/>
+    <hyperlink ref="E55" r:id="rId49" xr:uid="{A0BDFFED-5387-0F4C-9884-246C2DF53CD2}"/>
+    <hyperlink ref="E56" r:id="rId50" xr:uid="{D20543E9-DE50-EF44-ADCC-FE4E49F5B868}"/>
+    <hyperlink ref="E6" r:id="rId51" xr:uid="{D17F2BE4-9635-C146-8619-9BF315E32413}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
retira "global" de uma anotação
</commit_message>
<xml_diff>
--- a/R/dados_instrumentos.xlsx
+++ b/R/dados_instrumentos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiago/Documents/github/timeline-covid/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFFD5FC8-58BB-594E-85ED-07FDD88F2F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129E0DDF-5952-B643-8E04-75157CFD7E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-35500" yWindow="2280" windowWidth="25440" windowHeight="12820" xr2:uid="{69F0099A-28B2-B64C-97C8-E3F59C51DA57}"/>
   </bookViews>
@@ -651,9 +651,6 @@
     <t>Operação regresso de brasileiros no exterior</t>
   </si>
   <si>
-    <t>Aquisição de EPIs e capacitação para conter danos da pandemia global</t>
-  </si>
-  <si>
     <t>Auxílio Emergencial</t>
   </si>
   <si>
@@ -667,6 +664,9 @@
   </si>
   <si>
     <t>Auxílio Emergencial no valor de R$ 300</t>
+  </si>
+  <si>
+    <t>Aquisição de EPIs e capacitação para conter danos da pandemia</t>
   </si>
 </sst>
 </file>
@@ -1101,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7317090F-0B1F-F145-98D4-DA3D2D7A452A}">
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1193,7 +1193,7 @@
         <v>43923</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>21</v>
@@ -1342,7 +1342,7 @@
         <v>44021</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>35</v>
@@ -1365,7 +1365,7 @@
         <v>44076</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>37</v>
@@ -1770,7 +1770,7 @@
         <v>43978</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>90</v>
@@ -1837,7 +1837,7 @@
         <v>43903</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>119</v>
@@ -2156,7 +2156,7 @@
         <v>44049</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E49" s="8" t="s">
         <v>145</v>

</xml_diff>

<commit_message>
adiciona informação sobre a classificação do instrumento no Painel.
</commit_message>
<xml_diff>
--- a/R/dados_instrumentos.xlsx
+++ b/R/dados_instrumentos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiago/Documents/github/timeline-covid/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129E0DDF-5952-B643-8E04-75157CFD7E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FBB368C-F944-8E42-98A3-20046AC66689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35500" yWindow="2280" windowWidth="25440" windowHeight="12820" xr2:uid="{69F0099A-28B2-B64C-97C8-E3F59C51DA57}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" xr2:uid="{69F0099A-28B2-B64C-97C8-E3F59C51DA57}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="225">
   <si>
     <t>http://www.planalto.gov.br/CCIVIL_03/_Ato2019-2022/2020/Mpv/mpv929.htm</t>
   </si>
@@ -667,6 +667,48 @@
   </si>
   <si>
     <t>Aquisição de EPIs e capacitação para conter danos da pandemia</t>
+  </si>
+  <si>
+    <t>classificacao_painel</t>
+  </si>
+  <si>
+    <t>Auxílio Emergencial a pessoas em situação de vulnerabilidade, devido à pandemia da Covid-19</t>
+  </si>
+  <si>
+    <t>Transferência para a conta de Desenvolvimento Energético</t>
+  </si>
+  <si>
+    <t>Despesas Adicionais do Ministério da Saúde e demais ministérios</t>
+  </si>
+  <si>
+    <t>Auxílio Financeiro aos Estados, Municípios e DF</t>
+  </si>
+  <si>
+    <t>Benefício Emergencial de Manutenção do Emprego e Renda</t>
+  </si>
+  <si>
+    <t>Concessão de Financiamento para pagamento de folha salarial</t>
+  </si>
+  <si>
+    <t>Concessão de Financiamento para pagamento de folha salarial - Operacionalização financeira pela MP 943/2020</t>
+  </si>
+  <si>
+    <t>Financiamento de Infraestrutura Turística</t>
+  </si>
+  <si>
+    <t>Cotas dos Fundos Garantidores de Operações e de Crédito</t>
+  </si>
+  <si>
+    <t>Programa Emergencial de Acesso a Crédito - Maquininhas</t>
+  </si>
+  <si>
+    <t>Não está no Painel, pois trata apenas de regras. A operacionalização financeira foi feita pela MP nº 939/2020</t>
+  </si>
+  <si>
+    <t>Aquisição de Vacinas</t>
+  </si>
+  <si>
+    <t>Aquisição de Vacinas *reclassificado no Painel no dia 21 de junho de 2021</t>
   </si>
 </sst>
 </file>
@@ -1099,10 +1141,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7317090F-0B1F-F145-98D4-DA3D2D7A452A}">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1114,10 +1156,11 @@
     <col min="5" max="5" width="69.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="88" style="3" customWidth="1"/>
     <col min="7" max="7" width="86.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="8" max="8" width="62.5" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>199</v>
       </c>
@@ -1139,8 +1182,11 @@
       <c r="G1" s="3" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -1160,8 +1206,11 @@
       <c r="G2" s="7" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="H2" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -1181,8 +1230,11 @@
       <c r="G3" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H3" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -1204,8 +1256,11 @@
       <c r="G4" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H4" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -1225,8 +1280,11 @@
       <c r="G5" s="7" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="H5" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -1246,8 +1304,11 @@
       <c r="G6" s="7" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H6" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -1267,8 +1328,11 @@
       <c r="G7" s="10" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H7" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -1288,8 +1352,11 @@
       <c r="G8" s="10" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H8" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -1309,8 +1376,11 @@
       <c r="G9" s="10" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H9" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1330,8 +1400,11 @@
       <c r="G10" s="10" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H10" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1353,8 +1426,11 @@
       <c r="G11" s="10" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H11" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -1376,8 +1452,11 @@
       <c r="G12" s="10" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H12" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
@@ -1397,8 +1476,11 @@
       <c r="G13" s="10" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H13" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -1420,8 +1502,11 @@
       <c r="G14" s="10" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H14" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1441,8 +1526,11 @@
       <c r="G15" s="10" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H15" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>44</v>
       </c>
@@ -1464,8 +1552,11 @@
       <c r="G16" s="7" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H16" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>44</v>
       </c>
@@ -1485,8 +1576,11 @@
       <c r="G17" s="7" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H17" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>44</v>
       </c>
@@ -1506,8 +1600,11 @@
       <c r="G18" s="7" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H18" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>44</v>
       </c>
@@ -1527,8 +1624,11 @@
       <c r="G19" s="7" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H19" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>44</v>
       </c>
@@ -1548,8 +1648,11 @@
       <c r="G20" s="7" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H20" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>44</v>
       </c>
@@ -1569,8 +1672,11 @@
       <c r="G21" s="7" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H21" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>44</v>
       </c>
@@ -1590,8 +1696,11 @@
       <c r="G22" s="7" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H22" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>44</v>
       </c>
@@ -1611,8 +1720,11 @@
       <c r="G23" s="7" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H23" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>44</v>
       </c>
@@ -1632,8 +1744,11 @@
       <c r="G24" s="7" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H24" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>44</v>
       </c>
@@ -1653,8 +1768,11 @@
       <c r="G25" s="13" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H25" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>44</v>
       </c>
@@ -1674,8 +1792,11 @@
       <c r="G26" s="7" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H26" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>44</v>
       </c>
@@ -1695,8 +1816,11 @@
       <c r="G27" s="7" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H27" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>44</v>
       </c>
@@ -1716,8 +1840,11 @@
       <c r="G28" s="7" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="H28" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="85" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>81</v>
       </c>
@@ -1737,8 +1864,11 @@
       <c r="G29" s="10" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H29" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>81</v>
       </c>
@@ -1758,8 +1888,11 @@
       <c r="G30" s="10" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H30" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>81</v>
       </c>
@@ -1781,8 +1914,11 @@
       <c r="G31" s="10" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H31" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>81</v>
       </c>
@@ -1802,8 +1938,11 @@
       <c r="G32" s="10" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H32" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>94</v>
       </c>
@@ -1825,8 +1964,11 @@
       <c r="G33" s="7" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H33" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>94</v>
       </c>
@@ -1848,8 +1990,11 @@
       <c r="G34" s="7" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="H34" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>94</v>
       </c>
@@ -1871,8 +2016,11 @@
       <c r="G35" s="15" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H35" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
         <v>94</v>
       </c>
@@ -1892,8 +2040,11 @@
       <c r="G36" s="7" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H36" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>94</v>
       </c>
@@ -1913,8 +2064,11 @@
       <c r="G37" s="13" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="H37" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>94</v>
       </c>
@@ -1934,8 +2088,11 @@
       <c r="G38" s="13" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H38" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>94</v>
       </c>
@@ -1955,8 +2112,11 @@
       <c r="G39" s="7" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H39" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>94</v>
       </c>
@@ -1976,8 +2136,11 @@
       <c r="G40" s="13" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H40" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>94</v>
       </c>
@@ -1997,8 +2160,11 @@
       <c r="G41" s="15" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H41" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>94</v>
       </c>
@@ -2018,8 +2184,11 @@
       <c r="G42" s="7" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H42" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
         <v>94</v>
       </c>
@@ -2039,8 +2208,11 @@
       <c r="G43" s="7" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H43" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
         <v>94</v>
       </c>
@@ -2060,8 +2232,11 @@
       <c r="G44" s="7" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H44" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
         <v>94</v>
       </c>
@@ -2081,8 +2256,11 @@
       <c r="G45" s="7" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H45" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
         <v>94</v>
       </c>
@@ -2102,8 +2280,11 @@
       <c r="G46" s="7" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H46" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>94</v>
       </c>
@@ -2123,8 +2304,11 @@
       <c r="G47" s="7" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H47" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
         <v>94</v>
       </c>
@@ -2144,8 +2328,11 @@
       <c r="G48" s="7" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H48" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
         <v>94</v>
       </c>
@@ -2167,8 +2354,11 @@
       <c r="G49" s="7" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H49" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
         <v>94</v>
       </c>
@@ -2188,8 +2378,11 @@
       <c r="G50" s="7" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H50" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
         <v>94</v>
       </c>
@@ -2209,8 +2402,11 @@
       <c r="G51" s="7" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H51" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
         <v>94</v>
       </c>
@@ -2230,8 +2426,11 @@
       <c r="G52" s="7" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H52" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
         <v>94</v>
       </c>
@@ -2251,8 +2450,11 @@
       <c r="G53" s="7" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H53" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
         <v>94</v>
       </c>
@@ -2272,8 +2474,11 @@
       <c r="G54" s="7" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H54" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
         <v>94</v>
       </c>
@@ -2293,8 +2498,11 @@
       <c r="G55" s="7" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H55" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
         <v>94</v>
       </c>
@@ -2314,20 +2522,23 @@
       <c r="G56" s="7" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H56" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="7"/>
       <c r="B57" s="10"/>
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="7"/>
       <c r="B58" s="10"/>
       <c r="C58" s="9"/>
       <c r="D58" s="9"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="7"/>
       <c r="B59" s="10"/>
       <c r="C59" s="9"/>

</xml_diff>